<commit_message>
refatoração: gravação de análises
</commit_message>
<xml_diff>
--- a/dados/analises/2024/result/01-visao-geral/01-visao-geral.xlsx
+++ b/dados/analises/2024/result/01-visao-geral/01-visao-geral.xlsx
@@ -11,7 +11,7 @@
     <sheet name="plataforma" sheetId="2" r:id="rId2"/>
     <sheet name="uf" sheetId="3" r:id="rId3"/>
     <sheet name="classificacao_autoria" sheetId="4" r:id="rId4"/>
-    <sheet name="autor" sheetId="5" r:id="rId5"/>
+    <sheet name="autoria" sheetId="5" r:id="rId5"/>
     <sheet name="categoria" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -9759,7 +9759,7 @@
     <t>fabrizio andriani</t>
   </si>
   <si>
-    <t>categoria_mencao</t>
+    <t>categoria</t>
   </si>
   <si>
     <t>terror</t>

</xml_diff>